<commit_message>
some bug fixex, implemented multiprocesssing and added script for wrapping up label files
</commit_message>
<xml_diff>
--- a/workspace/datasets/merged_label_data.xlsx
+++ b/workspace/datasets/merged_label_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1232"/>
+  <dimension ref="A1:K1250"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14137,7 +14137,7 @@
       </c>
       <c r="K353" t="inlineStr">
         <is>
-          <t>INVERSE</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -14176,7 +14176,7 @@
       </c>
       <c r="K354" t="inlineStr">
         <is>
-          <t>INVERSE</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -14215,7 +14215,7 @@
       </c>
       <c r="K355" t="inlineStr">
         <is>
-          <t>INVERSE</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -22270,7 +22270,7 @@
       </c>
       <c r="K562" t="inlineStr">
         <is>
-          <t>INVERSE</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -22309,7 +22309,7 @@
       </c>
       <c r="K563" t="inlineStr">
         <is>
-          <t>INVERSE</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -22348,7 +22348,7 @@
       </c>
       <c r="K564" t="inlineStr">
         <is>
-          <t>INVERSE</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -22387,7 +22387,7 @@
       </c>
       <c r="K565" t="inlineStr">
         <is>
-          <t>INVERSE</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -22426,7 +22426,7 @@
       </c>
       <c r="K566" t="inlineStr">
         <is>
-          <t>INVERSE</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -35100,7 +35100,7 @@
       </c>
       <c r="K892" t="inlineStr">
         <is>
-          <t>INVERSE</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -45665,32 +45665,32 @@
       </c>
       <c r="B1168" t="inlineStr">
         <is>
-          <t>no_relative_sub_clauses_label=1_thresh=3</t>
+          <t>no_relative_clauses_label=1_thresh=8</t>
         </is>
       </c>
       <c r="C1168" t="n">
         <v>1</v>
       </c>
       <c r="D1168" t="n">
-        <v>0.142</v>
+        <v>0.06</v>
       </c>
       <c r="E1168" t="n">
-        <v>0.2</v>
+        <v>0.194</v>
       </c>
       <c r="F1168" t="n">
-        <v>0.584795321637427</v>
+        <v>0.7637795275590551</v>
       </c>
       <c r="G1168" t="n">
-        <v>0.415204678362573</v>
+        <v>0.2362204724409449</v>
       </c>
       <c r="H1168" t="n">
-        <v>0.342</v>
+        <v>0.254</v>
       </c>
       <c r="I1168" t="n">
-        <v>0.05800000000000002</v>
+        <v>0.134</v>
       </c>
       <c r="J1168" t="n">
-        <v>0.1695906432748539</v>
+        <v>0.5275590551181103</v>
       </c>
       <c r="K1168" t="inlineStr">
         <is>
@@ -45704,32 +45704,32 @@
       </c>
       <c r="B1169" t="inlineStr">
         <is>
-          <t>no_relative_sub_clauses_label=1_thresh=4</t>
+          <t>no_relative_clauses_label=1_thresh=9</t>
         </is>
       </c>
       <c r="C1169" t="n">
         <v>1</v>
       </c>
       <c r="D1169" t="n">
-        <v>0.122</v>
+        <v>0.046</v>
       </c>
       <c r="E1169" t="n">
-        <v>0.2</v>
+        <v>0.192</v>
       </c>
       <c r="F1169" t="n">
-        <v>0.6211180124223603</v>
+        <v>0.8067226890756303</v>
       </c>
       <c r="G1169" t="n">
-        <v>0.3788819875776397</v>
+        <v>0.1932773109243697</v>
       </c>
       <c r="H1169" t="n">
-        <v>0.322</v>
+        <v>0.238</v>
       </c>
       <c r="I1169" t="n">
-        <v>0.07800000000000001</v>
+        <v>0.146</v>
       </c>
       <c r="J1169" t="n">
-        <v>0.2422360248447205</v>
+        <v>0.6134453781512607</v>
       </c>
       <c r="K1169" t="inlineStr">
         <is>
@@ -45743,32 +45743,32 @@
       </c>
       <c r="B1170" t="inlineStr">
         <is>
-          <t>no_relative_sub_clauses_label=1_thresh=5</t>
+          <t>no_relative_clauses_label=1_thresh=10</t>
         </is>
       </c>
       <c r="C1170" t="n">
         <v>1</v>
       </c>
       <c r="D1170" t="n">
-        <v>0.092</v>
+        <v>0.026</v>
       </c>
       <c r="E1170" t="n">
-        <v>0.198</v>
+        <v>0.19</v>
       </c>
       <c r="F1170" t="n">
-        <v>0.6827586206896551</v>
+        <v>0.8796296296296297</v>
       </c>
       <c r="G1170" t="n">
-        <v>0.3172413793103449</v>
+        <v>0.1203703703703703</v>
       </c>
       <c r="H1170" t="n">
-        <v>0.29</v>
+        <v>0.216</v>
       </c>
       <c r="I1170" t="n">
-        <v>0.106</v>
+        <v>0.164</v>
       </c>
       <c r="J1170" t="n">
-        <v>0.3655172413793104</v>
+        <v>0.7592592592592593</v>
       </c>
       <c r="K1170" t="inlineStr">
         <is>
@@ -45782,32 +45782,32 @@
       </c>
       <c r="B1171" t="inlineStr">
         <is>
-          <t>no_relative_sub_clauses_label=1_thresh=6</t>
+          <t>no_relative_clauses_label=1_thresh=11</t>
         </is>
       </c>
       <c r="C1171" t="n">
         <v>1</v>
       </c>
       <c r="D1171" t="n">
-        <v>0.08</v>
+        <v>0.018</v>
       </c>
       <c r="E1171" t="n">
-        <v>0.196</v>
+        <v>0.188</v>
       </c>
       <c r="F1171" t="n">
-        <v>0.7101449275362318</v>
+        <v>0.912621359223301</v>
       </c>
       <c r="G1171" t="n">
-        <v>0.2898550724637682</v>
+        <v>0.08737864077669899</v>
       </c>
       <c r="H1171" t="n">
-        <v>0.276</v>
+        <v>0.206</v>
       </c>
       <c r="I1171" t="n">
-        <v>0.116</v>
+        <v>0.17</v>
       </c>
       <c r="J1171" t="n">
-        <v>0.4202898550724637</v>
+        <v>0.825242718446602</v>
       </c>
       <c r="K1171" t="inlineStr">
         <is>
@@ -45821,32 +45821,32 @@
       </c>
       <c r="B1172" t="inlineStr">
         <is>
-          <t>no_relative_sub_clauses_label=1_thresh=7</t>
+          <t>no_relative_clauses_label=1_thresh=12</t>
         </is>
       </c>
       <c r="C1172" t="n">
         <v>1</v>
       </c>
       <c r="D1172" t="n">
-        <v>0.076</v>
+        <v>0.014</v>
       </c>
       <c r="E1172" t="n">
-        <v>0.194</v>
+        <v>0.184</v>
       </c>
       <c r="F1172" t="n">
-        <v>0.7185185185185184</v>
+        <v>0.9292929292929293</v>
       </c>
       <c r="G1172" t="n">
-        <v>0.2814814814814816</v>
+        <v>0.07070707070707072</v>
       </c>
       <c r="H1172" t="n">
-        <v>0.27</v>
+        <v>0.198</v>
       </c>
       <c r="I1172" t="n">
-        <v>0.118</v>
+        <v>0.17</v>
       </c>
       <c r="J1172" t="n">
-        <v>0.4370370370370371</v>
+        <v>0.8585858585858585</v>
       </c>
       <c r="K1172" t="inlineStr">
         <is>
@@ -45860,32 +45860,32 @@
       </c>
       <c r="B1173" t="inlineStr">
         <is>
-          <t>avarage_distance_appearance_same_entities_paragraph_label=1_thresh=3</t>
+          <t>no_relative_sub_clauses_label=1_thresh=3</t>
         </is>
       </c>
       <c r="C1173" t="n">
         <v>1</v>
       </c>
       <c r="D1173" t="n">
-        <v>0.004</v>
+        <v>0.142</v>
       </c>
       <c r="E1173" t="n">
-        <v>0.034</v>
+        <v>0.2</v>
       </c>
       <c r="F1173" t="n">
-        <v>0.8947368421052631</v>
+        <v>0.584795321637427</v>
       </c>
       <c r="G1173" t="n">
-        <v>0.1052631578947369</v>
+        <v>0.415204678362573</v>
       </c>
       <c r="H1173" t="n">
-        <v>0.03800000000000001</v>
+        <v>0.342</v>
       </c>
       <c r="I1173" t="n">
-        <v>0.03</v>
+        <v>0.05800000000000002</v>
       </c>
       <c r="J1173" t="n">
-        <v>0.7894736842105262</v>
+        <v>0.1695906432748539</v>
       </c>
       <c r="K1173" t="inlineStr">
         <is>
@@ -45899,36 +45899,36 @@
       </c>
       <c r="B1174" t="inlineStr">
         <is>
-          <t>avarage_distance_appearance_same_entities_paragraph_label=1_thresh=4</t>
+          <t>no_relative_sub_clauses_label=1_thresh=4</t>
         </is>
       </c>
       <c r="C1174" t="n">
         <v>1</v>
       </c>
       <c r="D1174" t="n">
-        <v>0.004</v>
+        <v>0.122</v>
       </c>
       <c r="E1174" t="n">
-        <v>0.014</v>
+        <v>0.2</v>
       </c>
       <c r="F1174" t="n">
-        <v>0.7777777777777777</v>
+        <v>0.6211180124223603</v>
       </c>
       <c r="G1174" t="n">
-        <v>0.2222222222222223</v>
+        <v>0.3788819875776397</v>
       </c>
       <c r="H1174" t="n">
-        <v>0.018</v>
+        <v>0.322</v>
       </c>
       <c r="I1174" t="n">
-        <v>0.01</v>
+        <v>0.07800000000000001</v>
       </c>
       <c r="J1174" t="n">
-        <v>0.5555555555555555</v>
+        <v>0.2422360248447205</v>
       </c>
       <c r="K1174" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -45938,36 +45938,36 @@
       </c>
       <c r="B1175" t="inlineStr">
         <is>
-          <t>avarage_distance_appearance_same_entities_paragraph_label=1_thresh=5</t>
+          <t>no_relative_sub_clauses_label=1_thresh=5</t>
         </is>
       </c>
       <c r="C1175" t="n">
         <v>1</v>
       </c>
       <c r="D1175" t="n">
-        <v>0.002</v>
+        <v>0.092</v>
       </c>
       <c r="E1175" t="n">
-        <v>0.01</v>
+        <v>0.198</v>
       </c>
       <c r="F1175" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.6827586206896551</v>
       </c>
       <c r="G1175" t="n">
-        <v>0.1666666666666666</v>
+        <v>0.3172413793103449</v>
       </c>
       <c r="H1175" t="n">
-        <v>0.012</v>
+        <v>0.29</v>
       </c>
       <c r="I1175" t="n">
-        <v>0.008</v>
+        <v>0.106</v>
       </c>
       <c r="J1175" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.3655172413793104</v>
       </c>
       <c r="K1175" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -45977,36 +45977,36 @@
       </c>
       <c r="B1176" t="inlineStr">
         <is>
-          <t>avarage_distance_appearance_same_entities_paragraph_label=1_thresh=6</t>
+          <t>no_relative_sub_clauses_label=1_thresh=6</t>
         </is>
       </c>
       <c r="C1176" t="n">
         <v>1</v>
       </c>
       <c r="D1176" t="n">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="E1176" t="n">
-        <v>0.008</v>
+        <v>0.196</v>
       </c>
       <c r="F1176" t="n">
-        <v>1</v>
+        <v>0.7101449275362318</v>
       </c>
       <c r="G1176" t="n">
-        <v>0</v>
+        <v>0.2898550724637682</v>
       </c>
       <c r="H1176" t="n">
-        <v>0.008</v>
+        <v>0.276</v>
       </c>
       <c r="I1176" t="n">
-        <v>0.008</v>
+        <v>0.116</v>
       </c>
       <c r="J1176" t="n">
-        <v>1</v>
+        <v>0.4202898550724637</v>
       </c>
       <c r="K1176" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -46016,36 +46016,36 @@
       </c>
       <c r="B1177" t="inlineStr">
         <is>
-          <t>avarage_distance_appearance_same_entities_paragraph_label=1_thresh=7</t>
+          <t>no_relative_sub_clauses_label=1_thresh=7</t>
         </is>
       </c>
       <c r="C1177" t="n">
         <v>1</v>
       </c>
       <c r="D1177" t="n">
-        <v>0</v>
+        <v>0.076</v>
       </c>
       <c r="E1177" t="n">
-        <v>0.004</v>
+        <v>0.194</v>
       </c>
       <c r="F1177" t="n">
-        <v>1</v>
+        <v>0.7185185185185184</v>
       </c>
       <c r="G1177" t="n">
-        <v>0</v>
+        <v>0.2814814814814816</v>
       </c>
       <c r="H1177" t="n">
-        <v>0.004</v>
+        <v>0.27</v>
       </c>
       <c r="I1177" t="n">
-        <v>0.004</v>
+        <v>0.118</v>
       </c>
       <c r="J1177" t="n">
-        <v>1</v>
+        <v>0.4370370370370371</v>
       </c>
       <c r="K1177" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -46055,36 +46055,36 @@
       </c>
       <c r="B1178" t="inlineStr">
         <is>
-          <t>avarage_distance_appearance_same_entities_paragraph_label=1_thresh=8</t>
+          <t>no_relative_sub_clauses_label=1_thresh=8</t>
         </is>
       </c>
       <c r="C1178" t="n">
         <v>1</v>
       </c>
       <c r="D1178" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="E1178" t="n">
-        <v>0.004</v>
+        <v>0.194</v>
       </c>
       <c r="F1178" t="n">
-        <v>1</v>
+        <v>0.7637795275590551</v>
       </c>
       <c r="G1178" t="n">
-        <v>0</v>
+        <v>0.2362204724409449</v>
       </c>
       <c r="H1178" t="n">
-        <v>0.004</v>
+        <v>0.254</v>
       </c>
       <c r="I1178" t="n">
-        <v>0.004</v>
+        <v>0.134</v>
       </c>
       <c r="J1178" t="n">
-        <v>1</v>
+        <v>0.5275590551181103</v>
       </c>
       <c r="K1178" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -46094,36 +46094,36 @@
       </c>
       <c r="B1179" t="inlineStr">
         <is>
-          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=3</t>
+          <t>no_relative_sub_clauses_label=1_thresh=9</t>
         </is>
       </c>
       <c r="C1179" t="n">
         <v>1</v>
       </c>
       <c r="D1179" t="n">
-        <v>0.062</v>
+        <v>0.044</v>
       </c>
       <c r="E1179" t="n">
-        <v>0.004</v>
+        <v>0.192</v>
       </c>
       <c r="F1179" t="n">
-        <v>0.06060606060606061</v>
+        <v>0.8135593220338984</v>
       </c>
       <c r="G1179" t="n">
-        <v>0.9393939393939394</v>
+        <v>0.1864406779661016</v>
       </c>
       <c r="H1179" t="n">
-        <v>0.066</v>
+        <v>0.236</v>
       </c>
       <c r="I1179" t="n">
-        <v>0.058</v>
+        <v>0.148</v>
       </c>
       <c r="J1179" t="n">
-        <v>0.8787878787878787</v>
+        <v>0.6271186440677967</v>
       </c>
       <c r="K1179" t="inlineStr">
         <is>
-          <t>INVERSE</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -46133,36 +46133,36 @@
       </c>
       <c r="B1180" t="inlineStr">
         <is>
-          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=4</t>
+          <t>no_relative_sub_clauses_label=1_thresh=10</t>
         </is>
       </c>
       <c r="C1180" t="n">
         <v>1</v>
       </c>
       <c r="D1180" t="n">
-        <v>0.052</v>
+        <v>0.022</v>
       </c>
       <c r="E1180" t="n">
-        <v>0.004</v>
+        <v>0.19</v>
       </c>
       <c r="F1180" t="n">
-        <v>0.07142857142857144</v>
+        <v>0.8962264150943396</v>
       </c>
       <c r="G1180" t="n">
-        <v>0.9285714285714286</v>
+        <v>0.1037735849056604</v>
       </c>
       <c r="H1180" t="n">
-        <v>0.05599999999999999</v>
+        <v>0.212</v>
       </c>
       <c r="I1180" t="n">
-        <v>0.048</v>
+        <v>0.168</v>
       </c>
       <c r="J1180" t="n">
-        <v>0.8571428571428572</v>
+        <v>0.7924528301886793</v>
       </c>
       <c r="K1180" t="inlineStr">
         <is>
-          <t>INVERSE</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -46172,36 +46172,36 @@
       </c>
       <c r="B1181" t="inlineStr">
         <is>
-          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=5</t>
+          <t>no_relative_sub_clauses_label=1_thresh=11</t>
         </is>
       </c>
       <c r="C1181" t="n">
         <v>1</v>
       </c>
       <c r="D1181" t="n">
-        <v>0.04</v>
+        <v>0.018</v>
       </c>
       <c r="E1181" t="n">
-        <v>0.004</v>
+        <v>0.188</v>
       </c>
       <c r="F1181" t="n">
-        <v>0.09090909090909091</v>
+        <v>0.912621359223301</v>
       </c>
       <c r="G1181" t="n">
-        <v>0.9090909090909091</v>
+        <v>0.08737864077669899</v>
       </c>
       <c r="H1181" t="n">
-        <v>0.044</v>
+        <v>0.206</v>
       </c>
       <c r="I1181" t="n">
-        <v>0.036</v>
+        <v>0.17</v>
       </c>
       <c r="J1181" t="n">
-        <v>0.8181818181818183</v>
+        <v>0.825242718446602</v>
       </c>
       <c r="K1181" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -46211,36 +46211,36 @@
       </c>
       <c r="B1182" t="inlineStr">
         <is>
-          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=6</t>
+          <t>no_relative_sub_clauses_label=1_thresh=12</t>
         </is>
       </c>
       <c r="C1182" t="n">
         <v>1</v>
       </c>
       <c r="D1182" t="n">
-        <v>0.03</v>
+        <v>0.012</v>
       </c>
       <c r="E1182" t="n">
-        <v>0.004</v>
+        <v>0.184</v>
       </c>
       <c r="F1182" t="n">
-        <v>0.1176470588235294</v>
+        <v>0.9387755102040816</v>
       </c>
       <c r="G1182" t="n">
-        <v>0.8823529411764706</v>
+        <v>0.06122448979591844</v>
       </c>
       <c r="H1182" t="n">
-        <v>0.034</v>
+        <v>0.196</v>
       </c>
       <c r="I1182" t="n">
-        <v>0.026</v>
+        <v>0.172</v>
       </c>
       <c r="J1182" t="n">
-        <v>0.7647058823529411</v>
+        <v>0.8775510204081631</v>
       </c>
       <c r="K1182" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -46250,36 +46250,36 @@
       </c>
       <c r="B1183" t="inlineStr">
         <is>
-          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=7</t>
+          <t>avarage_distance_appearance_same_entities_paragraph_label=1_thresh=2</t>
         </is>
       </c>
       <c r="C1183" t="n">
         <v>1</v>
       </c>
       <c r="D1183" t="n">
-        <v>0.024</v>
+        <v>0.008</v>
       </c>
       <c r="E1183" t="n">
-        <v>0.004</v>
+        <v>0.052</v>
       </c>
       <c r="F1183" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="G1183" t="n">
-        <v>0.8571428571428572</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="H1183" t="n">
-        <v>0.028</v>
+        <v>0.06</v>
       </c>
       <c r="I1183" t="n">
-        <v>0.02</v>
+        <v>0.044</v>
       </c>
       <c r="J1183" t="n">
-        <v>0.7142857142857143</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="K1183" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -46289,36 +46289,36 @@
       </c>
       <c r="B1184" t="inlineStr">
         <is>
-          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=8</t>
+          <t>avarage_distance_appearance_same_entities_paragraph_label=1_thresh=2.5</t>
         </is>
       </c>
       <c r="C1184" t="n">
         <v>1</v>
       </c>
       <c r="D1184" t="n">
-        <v>0.024</v>
+        <v>0.008</v>
       </c>
       <c r="E1184" t="n">
-        <v>0.004</v>
+        <v>0.046</v>
       </c>
       <c r="F1184" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.8518518518518519</v>
       </c>
       <c r="G1184" t="n">
-        <v>0.8571428571428572</v>
+        <v>0.1481481481481481</v>
       </c>
       <c r="H1184" t="n">
-        <v>0.028</v>
+        <v>0.054</v>
       </c>
       <c r="I1184" t="n">
-        <v>0.02</v>
+        <v>0.038</v>
       </c>
       <c r="J1184" t="n">
-        <v>0.7142857142857143</v>
+        <v>0.7037037037037037</v>
       </c>
       <c r="K1184" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -46328,36 +46328,36 @@
       </c>
       <c r="B1185" t="inlineStr">
         <is>
-          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=9</t>
+          <t>avarage_distance_appearance_same_entities_paragraph_label=1_thresh=3</t>
         </is>
       </c>
       <c r="C1185" t="n">
         <v>1</v>
       </c>
       <c r="D1185" t="n">
-        <v>0.018</v>
+        <v>0.004</v>
       </c>
       <c r="E1185" t="n">
-        <v>0.004</v>
+        <v>0.034</v>
       </c>
       <c r="F1185" t="n">
-        <v>0.1818181818181818</v>
+        <v>0.8947368421052631</v>
       </c>
       <c r="G1185" t="n">
-        <v>0.8181818181818181</v>
+        <v>0.1052631578947369</v>
       </c>
       <c r="H1185" t="n">
-        <v>0.022</v>
+        <v>0.03800000000000001</v>
       </c>
       <c r="I1185" t="n">
-        <v>0.014</v>
+        <v>0.03</v>
       </c>
       <c r="J1185" t="n">
-        <v>0.6363636363636364</v>
+        <v>0.7894736842105262</v>
       </c>
       <c r="K1185" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -46367,23 +46367,23 @@
       </c>
       <c r="B1186" t="inlineStr">
         <is>
-          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=10</t>
+          <t>avarage_distance_appearance_same_entities_paragraph_label=1_thresh=4</t>
         </is>
       </c>
       <c r="C1186" t="n">
         <v>1</v>
       </c>
       <c r="D1186" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="E1186" t="n">
         <v>0.014</v>
       </c>
-      <c r="E1186" t="n">
-        <v>0.004</v>
-      </c>
       <c r="F1186" t="n">
-        <v>0.2222222222222222</v>
+        <v>0.7777777777777777</v>
       </c>
       <c r="G1186" t="n">
-        <v>0.7777777777777778</v>
+        <v>0.2222222222222223</v>
       </c>
       <c r="H1186" t="n">
         <v>0.018</v>
@@ -46406,32 +46406,32 @@
       </c>
       <c r="B1187" t="inlineStr">
         <is>
-          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=11</t>
+          <t>avarage_distance_appearance_same_entities_paragraph_label=1_thresh=5</t>
         </is>
       </c>
       <c r="C1187" t="n">
         <v>1</v>
       </c>
       <c r="D1187" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="E1187" t="n">
         <v>0.01</v>
       </c>
-      <c r="E1187" t="n">
-        <v>0.004</v>
-      </c>
       <c r="F1187" t="n">
-        <v>0.2857142857142857</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G1187" t="n">
-        <v>0.7142857142857143</v>
+        <v>0.1666666666666666</v>
       </c>
       <c r="H1187" t="n">
-        <v>0.014</v>
+        <v>0.012</v>
       </c>
       <c r="I1187" t="n">
-        <v>0.006</v>
+        <v>0.008</v>
       </c>
       <c r="J1187" t="n">
-        <v>0.4285714285714285</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="K1187" t="inlineStr">
         <is>
@@ -46445,32 +46445,32 @@
       </c>
       <c r="B1188" t="inlineStr">
         <is>
-          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=12</t>
+          <t>avarage_distance_appearance_same_entities_paragraph_label=1_thresh=6</t>
         </is>
       </c>
       <c r="C1188" t="n">
         <v>1</v>
       </c>
       <c r="D1188" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1188" t="n">
         <v>0.008</v>
       </c>
-      <c r="E1188" t="n">
-        <v>0.002</v>
-      </c>
       <c r="F1188" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="G1188" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="H1188" t="n">
-        <v>0.01</v>
+        <v>0.008</v>
       </c>
       <c r="I1188" t="n">
-        <v>0.006</v>
+        <v>0.008</v>
       </c>
       <c r="J1188" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="K1188" t="inlineStr">
         <is>
@@ -46484,32 +46484,32 @@
       </c>
       <c r="B1189" t="inlineStr">
         <is>
-          <t>low_num_words_in_sents_max_thres=20_label=1</t>
+          <t>avarage_distance_appearance_same_entities_paragraph_label=1_thresh=7</t>
         </is>
       </c>
       <c r="C1189" t="n">
         <v>1</v>
       </c>
       <c r="D1189" t="n">
-        <v>0.72</v>
+        <v>0</v>
       </c>
       <c r="E1189" t="n">
-        <v>0.726</v>
+        <v>0.004</v>
       </c>
       <c r="F1189" t="n">
-        <v>0.5020746887966805</v>
+        <v>1</v>
       </c>
       <c r="G1189" t="n">
-        <v>0.4979253112033195</v>
+        <v>0</v>
       </c>
       <c r="H1189" t="n">
-        <v>1.446</v>
+        <v>0.004</v>
       </c>
       <c r="I1189" t="n">
-        <v>0.006000000000000005</v>
+        <v>0.004</v>
       </c>
       <c r="J1189" t="n">
-        <v>0.004149377593360999</v>
+        <v>1</v>
       </c>
       <c r="K1189" t="inlineStr">
         <is>
@@ -46523,32 +46523,32 @@
       </c>
       <c r="B1190" t="inlineStr">
         <is>
-          <t>low_num_words_in_sents_max_thres=22_label=1</t>
+          <t>avarage_distance_appearance_same_entities_paragraph_label=1_thresh=8</t>
         </is>
       </c>
       <c r="C1190" t="n">
         <v>1</v>
       </c>
       <c r="D1190" t="n">
-        <v>0.646</v>
+        <v>0</v>
       </c>
       <c r="E1190" t="n">
-        <v>0.654</v>
+        <v>0.004</v>
       </c>
       <c r="F1190" t="n">
-        <v>0.5030769230769231</v>
+        <v>1</v>
       </c>
       <c r="G1190" t="n">
-        <v>0.4969230769230769</v>
+        <v>0</v>
       </c>
       <c r="H1190" t="n">
-        <v>1.3</v>
+        <v>0.004</v>
       </c>
       <c r="I1190" t="n">
-        <v>0.008000000000000007</v>
+        <v>0.004</v>
       </c>
       <c r="J1190" t="n">
-        <v>0.006153846153846159</v>
+        <v>1</v>
       </c>
       <c r="K1190" t="inlineStr">
         <is>
@@ -46562,32 +46562,32 @@
       </c>
       <c r="B1191" t="inlineStr">
         <is>
-          <t>low_num_words_in_sents_max_thres=24_label=1</t>
+          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=3</t>
         </is>
       </c>
       <c r="C1191" t="n">
         <v>1</v>
       </c>
       <c r="D1191" t="n">
-        <v>0.574</v>
+        <v>0.062</v>
       </c>
       <c r="E1191" t="n">
-        <v>0.6</v>
+        <v>0.004</v>
       </c>
       <c r="F1191" t="n">
-        <v>0.5110732538330495</v>
+        <v>0.06060606060606061</v>
       </c>
       <c r="G1191" t="n">
-        <v>0.4889267461669505</v>
+        <v>0.9393939393939394</v>
       </c>
       <c r="H1191" t="n">
-        <v>1.174</v>
+        <v>0.066</v>
       </c>
       <c r="I1191" t="n">
-        <v>0.02600000000000002</v>
+        <v>0.058</v>
       </c>
       <c r="J1191" t="n">
-        <v>0.02214650766609883</v>
+        <v>0.8787878787878787</v>
       </c>
       <c r="K1191" t="inlineStr">
         <is>
@@ -46601,36 +46601,36 @@
       </c>
       <c r="B1192" t="inlineStr">
         <is>
-          <t>low_num_words_in_sents_max_thres=26_label=1</t>
+          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=4</t>
         </is>
       </c>
       <c r="C1192" t="n">
         <v>1</v>
       </c>
       <c r="D1192" t="n">
-        <v>0.504</v>
+        <v>0.052</v>
       </c>
       <c r="E1192" t="n">
-        <v>0.5639999999999999</v>
+        <v>0.004</v>
       </c>
       <c r="F1192" t="n">
-        <v>0.5280898876404494</v>
+        <v>0.07142857142857144</v>
       </c>
       <c r="G1192" t="n">
-        <v>0.4719101123595506</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="H1192" t="n">
-        <v>1.068</v>
+        <v>0.05599999999999999</v>
       </c>
       <c r="I1192" t="n">
-        <v>0.05999999999999994</v>
+        <v>0.048</v>
       </c>
       <c r="J1192" t="n">
-        <v>0.05617977528089882</v>
+        <v>0.8571428571428572</v>
       </c>
       <c r="K1192" t="inlineStr">
         <is>
-          <t>JA</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -46640,36 +46640,36 @@
       </c>
       <c r="B1193" t="inlineStr">
         <is>
-          <t>low_num_words_in_sents_max_thres=28_label=1</t>
+          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=5</t>
         </is>
       </c>
       <c r="C1193" t="n">
         <v>1</v>
       </c>
       <c r="D1193" t="n">
-        <v>0.432</v>
+        <v>0.04</v>
       </c>
       <c r="E1193" t="n">
-        <v>0.496</v>
+        <v>0.004</v>
       </c>
       <c r="F1193" t="n">
-        <v>0.5344827586206897</v>
+        <v>0.09090909090909091</v>
       </c>
       <c r="G1193" t="n">
-        <v>0.4655172413793103</v>
+        <v>0.9090909090909091</v>
       </c>
       <c r="H1193" t="n">
-        <v>0.9279999999999999</v>
+        <v>0.044</v>
       </c>
       <c r="I1193" t="n">
-        <v>0.064</v>
+        <v>0.036</v>
       </c>
       <c r="J1193" t="n">
-        <v>0.06896551724137932</v>
+        <v>0.8181818181818183</v>
       </c>
       <c r="K1193" t="inlineStr">
         <is>
-          <t>JA</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -46679,36 +46679,36 @@
       </c>
       <c r="B1194" t="inlineStr">
         <is>
-          <t>low_num_words_in_sents_max_thres=30_label=1</t>
+          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=6</t>
         </is>
       </c>
       <c r="C1194" t="n">
         <v>1</v>
       </c>
       <c r="D1194" t="n">
-        <v>0.376</v>
+        <v>0.03</v>
       </c>
       <c r="E1194" t="n">
-        <v>0.446</v>
+        <v>0.004</v>
       </c>
       <c r="F1194" t="n">
-        <v>0.5425790754257908</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="G1194" t="n">
-        <v>0.4574209245742092</v>
+        <v>0.8823529411764706</v>
       </c>
       <c r="H1194" t="n">
-        <v>0.8220000000000001</v>
+        <v>0.034</v>
       </c>
       <c r="I1194" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.026</v>
       </c>
       <c r="J1194" t="n">
-        <v>0.08515815085158152</v>
+        <v>0.7647058823529411</v>
       </c>
       <c r="K1194" t="inlineStr">
         <is>
-          <t>JA</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -46718,36 +46718,36 @@
       </c>
       <c r="B1195" t="inlineStr">
         <is>
-          <t>low_num_words_in_sents_max_thres=35_label=1</t>
+          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=7</t>
         </is>
       </c>
       <c r="C1195" t="n">
         <v>1</v>
       </c>
       <c r="D1195" t="n">
-        <v>0.294</v>
+        <v>0.024</v>
       </c>
       <c r="E1195" t="n">
-        <v>0.362</v>
+        <v>0.004</v>
       </c>
       <c r="F1195" t="n">
-        <v>0.551829268292683</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="G1195" t="n">
-        <v>0.448170731707317</v>
+        <v>0.8571428571428572</v>
       </c>
       <c r="H1195" t="n">
-        <v>0.6559999999999999</v>
+        <v>0.028</v>
       </c>
       <c r="I1195" t="n">
-        <v>0.068</v>
+        <v>0.02</v>
       </c>
       <c r="J1195" t="n">
-        <v>0.1036585365853659</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="K1195" t="inlineStr">
         <is>
-          <t>JA</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -46757,36 +46757,36 @@
       </c>
       <c r="B1196" t="inlineStr">
         <is>
-          <t>low_num_words_in_sents_max_thres=40_label=1</t>
+          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=8</t>
         </is>
       </c>
       <c r="C1196" t="n">
         <v>1</v>
       </c>
       <c r="D1196" t="n">
-        <v>0.222</v>
+        <v>0.024</v>
       </c>
       <c r="E1196" t="n">
-        <v>0.3</v>
+        <v>0.004</v>
       </c>
       <c r="F1196" t="n">
-        <v>0.5747126436781609</v>
+        <v>0.1428571428571428</v>
       </c>
       <c r="G1196" t="n">
-        <v>0.4252873563218391</v>
+        <v>0.8571428571428572</v>
       </c>
       <c r="H1196" t="n">
-        <v>0.522</v>
+        <v>0.028</v>
       </c>
       <c r="I1196" t="n">
-        <v>0.07799999999999999</v>
+        <v>0.02</v>
       </c>
       <c r="J1196" t="n">
-        <v>0.1494252873563218</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="K1196" t="inlineStr">
         <is>
-          <t>JA</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -46796,36 +46796,36 @@
       </c>
       <c r="B1197" t="inlineStr">
         <is>
-          <t>low_num_words_in_sents_avg_thres=20_label=1</t>
+          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=9</t>
         </is>
       </c>
       <c r="C1197" t="n">
         <v>1</v>
       </c>
       <c r="D1197" t="n">
-        <v>0.588</v>
+        <v>0.018</v>
       </c>
       <c r="E1197" t="n">
-        <v>0.656</v>
+        <v>0.004</v>
       </c>
       <c r="F1197" t="n">
-        <v>0.527331189710611</v>
+        <v>0.1818181818181818</v>
       </c>
       <c r="G1197" t="n">
-        <v>0.472668810289389</v>
+        <v>0.8181818181818181</v>
       </c>
       <c r="H1197" t="n">
-        <v>1.244</v>
+        <v>0.022</v>
       </c>
       <c r="I1197" t="n">
-        <v>0.06800000000000006</v>
+        <v>0.014</v>
       </c>
       <c r="J1197" t="n">
-        <v>0.05466237942122192</v>
+        <v>0.6363636363636364</v>
       </c>
       <c r="K1197" t="inlineStr">
         <is>
-          <t>JA</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -46835,36 +46835,36 @@
       </c>
       <c r="B1198" t="inlineStr">
         <is>
-          <t>low_num_words_in_sents_avg_thres=22_label=1</t>
+          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=10</t>
         </is>
       </c>
       <c r="C1198" t="n">
         <v>1</v>
       </c>
       <c r="D1198" t="n">
-        <v>0.466</v>
+        <v>0.014</v>
       </c>
       <c r="E1198" t="n">
-        <v>0.534</v>
+        <v>0.004</v>
       </c>
       <c r="F1198" t="n">
-        <v>0.534</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="G1198" t="n">
-        <v>0.466</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="H1198" t="n">
-        <v>1</v>
+        <v>0.018</v>
       </c>
       <c r="I1198" t="n">
-        <v>0.068</v>
+        <v>0.01</v>
       </c>
       <c r="J1198" t="n">
-        <v>0.068</v>
+        <v>0.5555555555555555</v>
       </c>
       <c r="K1198" t="inlineStr">
         <is>
-          <t>JA</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -46874,36 +46874,36 @@
       </c>
       <c r="B1199" t="inlineStr">
         <is>
-          <t>low_num_words_in_sents_avg_thres=24_label=1</t>
+          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=11</t>
         </is>
       </c>
       <c r="C1199" t="n">
         <v>1</v>
       </c>
       <c r="D1199" t="n">
-        <v>0.346</v>
+        <v>0.01</v>
       </c>
       <c r="E1199" t="n">
-        <v>0.424</v>
+        <v>0.004</v>
       </c>
       <c r="F1199" t="n">
-        <v>0.5506493506493506</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="G1199" t="n">
-        <v>0.4493506493506494</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="H1199" t="n">
-        <v>0.77</v>
+        <v>0.014</v>
       </c>
       <c r="I1199" t="n">
-        <v>0.07800000000000001</v>
+        <v>0.006</v>
       </c>
       <c r="J1199" t="n">
-        <v>0.1012987012987013</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="K1199" t="inlineStr">
         <is>
-          <t>JA</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -46913,36 +46913,36 @@
       </c>
       <c r="B1200" t="inlineStr">
         <is>
-          <t>low_num_words_in_sents_avg_thres=26_label=1</t>
+          <t>avarage_distance_appearance_same_entities_sentence_label=1_thresh=12</t>
         </is>
       </c>
       <c r="C1200" t="n">
         <v>1</v>
       </c>
       <c r="D1200" t="n">
-        <v>0.26</v>
+        <v>0.008</v>
       </c>
       <c r="E1200" t="n">
-        <v>0.344</v>
+        <v>0.002</v>
       </c>
       <c r="F1200" t="n">
-        <v>0.5695364238410596</v>
+        <v>0.2</v>
       </c>
       <c r="G1200" t="n">
-        <v>0.4304635761589404</v>
+        <v>0.8</v>
       </c>
       <c r="H1200" t="n">
-        <v>0.604</v>
+        <v>0.01</v>
       </c>
       <c r="I1200" t="n">
-        <v>0.08399999999999996</v>
+        <v>0.006</v>
       </c>
       <c r="J1200" t="n">
-        <v>0.1390728476821191</v>
+        <v>0.6</v>
       </c>
       <c r="K1200" t="inlineStr">
         <is>
-          <t>JA</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -46952,36 +46952,36 @@
       </c>
       <c r="B1201" t="inlineStr">
         <is>
-          <t>low_num_words_in_sents_avg_thres=28_label=1</t>
+          <t>low_num_words_in_sents_max_thres=20_label=1</t>
         </is>
       </c>
       <c r="C1201" t="n">
         <v>1</v>
       </c>
       <c r="D1201" t="n">
-        <v>0.202</v>
+        <v>0.72</v>
       </c>
       <c r="E1201" t="n">
-        <v>0.25</v>
+        <v>0.726</v>
       </c>
       <c r="F1201" t="n">
-        <v>0.5530973451327433</v>
+        <v>0.5020746887966805</v>
       </c>
       <c r="G1201" t="n">
-        <v>0.4469026548672567</v>
+        <v>0.4979253112033195</v>
       </c>
       <c r="H1201" t="n">
-        <v>0.452</v>
+        <v>1.446</v>
       </c>
       <c r="I1201" t="n">
-        <v>0.04799999999999999</v>
+        <v>0.006000000000000005</v>
       </c>
       <c r="J1201" t="n">
-        <v>0.1061946902654867</v>
+        <v>0.004149377593360999</v>
       </c>
       <c r="K1201" t="inlineStr">
         <is>
-          <t>JA</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -46991,36 +46991,36 @@
       </c>
       <c r="B1202" t="inlineStr">
         <is>
-          <t>low_num_words_in_sents_avg_thres=30_label=1</t>
+          <t>low_num_words_in_sents_max_thres=22_label=1</t>
         </is>
       </c>
       <c r="C1202" t="n">
         <v>1</v>
       </c>
       <c r="D1202" t="n">
-        <v>0.136</v>
+        <v>0.646</v>
       </c>
       <c r="E1202" t="n">
-        <v>0.194</v>
+        <v>0.654</v>
       </c>
       <c r="F1202" t="n">
-        <v>0.5878787878787879</v>
+        <v>0.5030769230769231</v>
       </c>
       <c r="G1202" t="n">
-        <v>0.4121212121212121</v>
+        <v>0.4969230769230769</v>
       </c>
       <c r="H1202" t="n">
-        <v>0.33</v>
+        <v>1.3</v>
       </c>
       <c r="I1202" t="n">
-        <v>0.058</v>
+        <v>0.008000000000000007</v>
       </c>
       <c r="J1202" t="n">
-        <v>0.1757575757575757</v>
+        <v>0.006153846153846159</v>
       </c>
       <c r="K1202" t="inlineStr">
         <is>
-          <t>JA</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -47030,36 +47030,36 @@
       </c>
       <c r="B1203" t="inlineStr">
         <is>
-          <t>low_num_words_in_sents_avg_thres=35_label=1</t>
+          <t>low_num_words_in_sents_max_thres=24_label=1</t>
         </is>
       </c>
       <c r="C1203" t="n">
         <v>1</v>
       </c>
       <c r="D1203" t="n">
-        <v>0.068</v>
+        <v>0.574</v>
       </c>
       <c r="E1203" t="n">
-        <v>0.114</v>
+        <v>0.6</v>
       </c>
       <c r="F1203" t="n">
-        <v>0.6263736263736264</v>
+        <v>0.5110732538330495</v>
       </c>
       <c r="G1203" t="n">
-        <v>0.3736263736263736</v>
+        <v>0.4889267461669505</v>
       </c>
       <c r="H1203" t="n">
-        <v>0.182</v>
+        <v>1.174</v>
       </c>
       <c r="I1203" t="n">
-        <v>0.046</v>
+        <v>0.02600000000000002</v>
       </c>
       <c r="J1203" t="n">
-        <v>0.2527472527472527</v>
+        <v>0.02214650766609883</v>
       </c>
       <c r="K1203" t="inlineStr">
         <is>
-          <t>JA</t>
+          <t>NEIN</t>
         </is>
       </c>
     </row>
@@ -47069,32 +47069,32 @@
       </c>
       <c r="B1204" t="inlineStr">
         <is>
-          <t>low_num_words_in_sents_avg_thres=40_label=1</t>
+          <t>low_num_words_in_sents_max_thres=26_label=1</t>
         </is>
       </c>
       <c r="C1204" t="n">
         <v>1</v>
       </c>
       <c r="D1204" t="n">
-        <v>0.034</v>
+        <v>0.504</v>
       </c>
       <c r="E1204" t="n">
-        <v>0.068</v>
+        <v>0.5639999999999999</v>
       </c>
       <c r="F1204" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5280898876404494</v>
       </c>
       <c r="G1204" t="n">
-        <v>0.3333333333333334</v>
+        <v>0.4719101123595506</v>
       </c>
       <c r="H1204" t="n">
-        <v>0.102</v>
+        <v>1.068</v>
       </c>
       <c r="I1204" t="n">
-        <v>0.034</v>
+        <v>0.05999999999999994</v>
       </c>
       <c r="J1204" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.05617977528089882</v>
       </c>
       <c r="K1204" t="inlineStr">
         <is>
@@ -47108,36 +47108,36 @@
       </c>
       <c r="B1205" t="inlineStr">
         <is>
-          <t>num_sents_num_thres=5_label=1</t>
+          <t>low_num_words_in_sents_max_thres=28_label=1</t>
         </is>
       </c>
       <c r="C1205" t="n">
         <v>1</v>
       </c>
       <c r="D1205" t="n">
-        <v>0.208</v>
+        <v>0.432</v>
       </c>
       <c r="E1205" t="n">
-        <v>0.208</v>
+        <v>0.496</v>
       </c>
       <c r="F1205" t="n">
-        <v>0.5</v>
+        <v>0.5344827586206897</v>
       </c>
       <c r="G1205" t="n">
-        <v>0.5</v>
+        <v>0.4655172413793103</v>
       </c>
       <c r="H1205" t="n">
-        <v>0.416</v>
+        <v>0.9279999999999999</v>
       </c>
       <c r="I1205" t="n">
-        <v>0</v>
+        <v>0.064</v>
       </c>
       <c r="J1205" t="n">
-        <v>0</v>
+        <v>0.06896551724137932</v>
       </c>
       <c r="K1205" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -47147,36 +47147,36 @@
       </c>
       <c r="B1206" t="inlineStr">
         <is>
-          <t>num_sents_num_thres=6_label=1</t>
+          <t>low_num_words_in_sents_max_thres=30_label=1</t>
         </is>
       </c>
       <c r="C1206" t="n">
         <v>1</v>
       </c>
       <c r="D1206" t="n">
-        <v>0.206</v>
+        <v>0.376</v>
       </c>
       <c r="E1206" t="n">
-        <v>0.208</v>
+        <v>0.446</v>
       </c>
       <c r="F1206" t="n">
-        <v>0.5024154589371981</v>
+        <v>0.5425790754257908</v>
       </c>
       <c r="G1206" t="n">
-        <v>0.4975845410628019</v>
+        <v>0.4574209245742092</v>
       </c>
       <c r="H1206" t="n">
-        <v>0.414</v>
+        <v>0.8220000000000001</v>
       </c>
       <c r="I1206" t="n">
-        <v>0.002000000000000002</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="J1206" t="n">
-        <v>0.004830917874396139</v>
+        <v>0.08515815085158152</v>
       </c>
       <c r="K1206" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -47186,36 +47186,36 @@
       </c>
       <c r="B1207" t="inlineStr">
         <is>
-          <t>num_sents_num_thres=7_label=1</t>
+          <t>low_num_words_in_sents_max_thres=35_label=1</t>
         </is>
       </c>
       <c r="C1207" t="n">
         <v>1</v>
       </c>
       <c r="D1207" t="n">
-        <v>0.202</v>
+        <v>0.294</v>
       </c>
       <c r="E1207" t="n">
-        <v>0.204</v>
+        <v>0.362</v>
       </c>
       <c r="F1207" t="n">
-        <v>0.5024630541871921</v>
+        <v>0.551829268292683</v>
       </c>
       <c r="G1207" t="n">
-        <v>0.4975369458128079</v>
+        <v>0.448170731707317</v>
       </c>
       <c r="H1207" t="n">
-        <v>0.406</v>
+        <v>0.6559999999999999</v>
       </c>
       <c r="I1207" t="n">
-        <v>0.001999999999999974</v>
+        <v>0.068</v>
       </c>
       <c r="J1207" t="n">
-        <v>0.004926108374384172</v>
+        <v>0.1036585365853659</v>
       </c>
       <c r="K1207" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -47225,36 +47225,36 @@
       </c>
       <c r="B1208" t="inlineStr">
         <is>
-          <t>num_sents_num_thres=8_label=1</t>
+          <t>low_num_words_in_sents_max_thres=40_label=1</t>
         </is>
       </c>
       <c r="C1208" t="n">
         <v>1</v>
       </c>
       <c r="D1208" t="n">
-        <v>0.202</v>
+        <v>0.222</v>
       </c>
       <c r="E1208" t="n">
-        <v>0.204</v>
+        <v>0.3</v>
       </c>
       <c r="F1208" t="n">
-        <v>0.5024630541871921</v>
+        <v>0.5747126436781609</v>
       </c>
       <c r="G1208" t="n">
-        <v>0.4975369458128079</v>
+        <v>0.4252873563218391</v>
       </c>
       <c r="H1208" t="n">
-        <v>0.406</v>
+        <v>0.522</v>
       </c>
       <c r="I1208" t="n">
-        <v>0.001999999999999974</v>
+        <v>0.07799999999999999</v>
       </c>
       <c r="J1208" t="n">
-        <v>0.004926108374384172</v>
+        <v>0.1494252873563218</v>
       </c>
       <c r="K1208" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -47264,36 +47264,36 @@
       </c>
       <c r="B1209" t="inlineStr">
         <is>
-          <t>num_sents_num_thres=9_label=1</t>
+          <t>low_num_words_in_sents_max_thres=42_label=1</t>
         </is>
       </c>
       <c r="C1209" t="n">
         <v>1</v>
       </c>
       <c r="D1209" t="n">
-        <v>0.202</v>
+        <v>0.2</v>
       </c>
       <c r="E1209" t="n">
-        <v>0.204</v>
+        <v>0.276</v>
       </c>
       <c r="F1209" t="n">
-        <v>0.5024630541871921</v>
+        <v>0.5798319327731093</v>
       </c>
       <c r="G1209" t="n">
-        <v>0.4975369458128079</v>
+        <v>0.4201680672268907</v>
       </c>
       <c r="H1209" t="n">
-        <v>0.406</v>
+        <v>0.476</v>
       </c>
       <c r="I1209" t="n">
-        <v>0.001999999999999974</v>
+        <v>0.07600000000000001</v>
       </c>
       <c r="J1209" t="n">
-        <v>0.004926108374384172</v>
+        <v>0.1596638655462185</v>
       </c>
       <c r="K1209" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -47303,36 +47303,36 @@
       </c>
       <c r="B1210" t="inlineStr">
         <is>
-          <t>num_sents_num_thres=10_label=1</t>
+          <t>low_num_words_in_sents_max_thres=45_label=1</t>
         </is>
       </c>
       <c r="C1210" t="n">
         <v>1</v>
       </c>
       <c r="D1210" t="n">
-        <v>0.196</v>
+        <v>0.162</v>
       </c>
       <c r="E1210" t="n">
-        <v>0.204</v>
+        <v>0.26</v>
       </c>
       <c r="F1210" t="n">
-        <v>0.5099999999999999</v>
+        <v>0.6161137440758293</v>
       </c>
       <c r="G1210" t="n">
-        <v>0.4900000000000001</v>
+        <v>0.3838862559241707</v>
       </c>
       <c r="H1210" t="n">
-        <v>0.4</v>
+        <v>0.422</v>
       </c>
       <c r="I1210" t="n">
-        <v>0.007999999999999979</v>
+        <v>0.098</v>
       </c>
       <c r="J1210" t="n">
-        <v>0.01999999999999995</v>
+        <v>0.2322274881516588</v>
       </c>
       <c r="K1210" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -47342,36 +47342,36 @@
       </c>
       <c r="B1211" t="inlineStr">
         <is>
-          <t>num_sents_num_thres=11_label=1</t>
+          <t>low_num_words_in_sents_max_thres=50_label=1</t>
         </is>
       </c>
       <c r="C1211" t="n">
         <v>1</v>
       </c>
       <c r="D1211" t="n">
-        <v>0.194</v>
+        <v>0.112</v>
       </c>
       <c r="E1211" t="n">
-        <v>0.204</v>
+        <v>0.222</v>
       </c>
       <c r="F1211" t="n">
-        <v>0.5125628140703516</v>
+        <v>0.6646706586826348</v>
       </c>
       <c r="G1211" t="n">
-        <v>0.4874371859296484</v>
+        <v>0.3353293413173652</v>
       </c>
       <c r="H1211" t="n">
-        <v>0.398</v>
+        <v>0.334</v>
       </c>
       <c r="I1211" t="n">
-        <v>0.009999999999999981</v>
+        <v>0.11</v>
       </c>
       <c r="J1211" t="n">
-        <v>0.02512562814070347</v>
+        <v>0.3293413173652694</v>
       </c>
       <c r="K1211" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -47381,36 +47381,36 @@
       </c>
       <c r="B1212" t="inlineStr">
         <is>
-          <t>few_modifiers_thres=5_label=1</t>
+          <t>low_num_words_in_sents_avg_thres=20_label=1</t>
         </is>
       </c>
       <c r="C1212" t="n">
         <v>1</v>
       </c>
       <c r="D1212" t="n">
-        <v>0.432</v>
+        <v>0.588</v>
       </c>
       <c r="E1212" t="n">
-        <v>0.414</v>
+        <v>0.656</v>
       </c>
       <c r="F1212" t="n">
-        <v>0.4893617021276596</v>
+        <v>0.527331189710611</v>
       </c>
       <c r="G1212" t="n">
-        <v>0.5106382978723405</v>
+        <v>0.472668810289389</v>
       </c>
       <c r="H1212" t="n">
-        <v>0.846</v>
+        <v>1.244</v>
       </c>
       <c r="I1212" t="n">
-        <v>0.01800000000000002</v>
+        <v>0.06800000000000006</v>
       </c>
       <c r="J1212" t="n">
-        <v>0.02127659574468087</v>
+        <v>0.05466237942122192</v>
       </c>
       <c r="K1212" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -47420,36 +47420,36 @@
       </c>
       <c r="B1213" t="inlineStr">
         <is>
-          <t>few_modifiers_thres=6_label=1</t>
+          <t>low_num_words_in_sents_avg_thres=22_label=1</t>
         </is>
       </c>
       <c r="C1213" t="n">
         <v>1</v>
       </c>
       <c r="D1213" t="n">
-        <v>0.364</v>
+        <v>0.466</v>
       </c>
       <c r="E1213" t="n">
-        <v>0.354</v>
+        <v>0.534</v>
       </c>
       <c r="F1213" t="n">
-        <v>0.4930362116991643</v>
+        <v>0.534</v>
       </c>
       <c r="G1213" t="n">
-        <v>0.5069637883008357</v>
+        <v>0.466</v>
       </c>
       <c r="H1213" t="n">
-        <v>0.718</v>
+        <v>1</v>
       </c>
       <c r="I1213" t="n">
-        <v>0.01000000000000001</v>
+        <v>0.068</v>
       </c>
       <c r="J1213" t="n">
-        <v>0.01392757660167132</v>
+        <v>0.068</v>
       </c>
       <c r="K1213" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -47459,36 +47459,36 @@
       </c>
       <c r="B1214" t="inlineStr">
         <is>
-          <t>few_modifiers_thres=7_label=1</t>
+          <t>low_num_words_in_sents_avg_thres=24_label=1</t>
         </is>
       </c>
       <c r="C1214" t="n">
         <v>1</v>
       </c>
       <c r="D1214" t="n">
-        <v>0.32</v>
+        <v>0.346</v>
       </c>
       <c r="E1214" t="n">
-        <v>0.324</v>
+        <v>0.424</v>
       </c>
       <c r="F1214" t="n">
-        <v>0.5031055900621118</v>
+        <v>0.5506493506493506</v>
       </c>
       <c r="G1214" t="n">
-        <v>0.4968944099378882</v>
+        <v>0.4493506493506494</v>
       </c>
       <c r="H1214" t="n">
-        <v>0.644</v>
+        <v>0.77</v>
       </c>
       <c r="I1214" t="n">
-        <v>0.004000000000000004</v>
+        <v>0.07800000000000001</v>
       </c>
       <c r="J1214" t="n">
-        <v>0.006211180124223608</v>
+        <v>0.1012987012987013</v>
       </c>
       <c r="K1214" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -47498,36 +47498,36 @@
       </c>
       <c r="B1215" t="inlineStr">
         <is>
-          <t>few_modifiers_thres=8_label=1</t>
+          <t>low_num_words_in_sents_avg_thres=26_label=1</t>
         </is>
       </c>
       <c r="C1215" t="n">
         <v>1</v>
       </c>
       <c r="D1215" t="n">
-        <v>0.296</v>
+        <v>0.26</v>
       </c>
       <c r="E1215" t="n">
-        <v>0.304</v>
+        <v>0.344</v>
       </c>
       <c r="F1215" t="n">
-        <v>0.5066666666666667</v>
+        <v>0.5695364238410596</v>
       </c>
       <c r="G1215" t="n">
-        <v>0.4933333333333333</v>
+        <v>0.4304635761589404</v>
       </c>
       <c r="H1215" t="n">
-        <v>0.6</v>
+        <v>0.604</v>
       </c>
       <c r="I1215" t="n">
-        <v>0.008000000000000007</v>
+        <v>0.08399999999999996</v>
       </c>
       <c r="J1215" t="n">
-        <v>0.01333333333333335</v>
+        <v>0.1390728476821191</v>
       </c>
       <c r="K1215" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -47537,36 +47537,36 @@
       </c>
       <c r="B1216" t="inlineStr">
         <is>
-          <t>few_modifiers_thres=9_label=1</t>
+          <t>low_num_words_in_sents_avg_thres=28_label=1</t>
         </is>
       </c>
       <c r="C1216" t="n">
         <v>1</v>
       </c>
       <c r="D1216" t="n">
-        <v>0.27</v>
+        <v>0.202</v>
       </c>
       <c r="E1216" t="n">
-        <v>0.276</v>
+        <v>0.25</v>
       </c>
       <c r="F1216" t="n">
-        <v>0.5054945054945055</v>
+        <v>0.5530973451327433</v>
       </c>
       <c r="G1216" t="n">
-        <v>0.4945054945054945</v>
+        <v>0.4469026548672567</v>
       </c>
       <c r="H1216" t="n">
-        <v>0.546</v>
+        <v>0.452</v>
       </c>
       <c r="I1216" t="n">
-        <v>0.006000000000000005</v>
+        <v>0.04799999999999999</v>
       </c>
       <c r="J1216" t="n">
-        <v>0.010989010989011</v>
+        <v>0.1061946902654867</v>
       </c>
       <c r="K1216" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -47576,36 +47576,36 @@
       </c>
       <c r="B1217" t="inlineStr">
         <is>
-          <t>few_modifiers_thres=10_label=1</t>
+          <t>low_num_words_in_sents_avg_thres=30_label=1</t>
         </is>
       </c>
       <c r="C1217" t="n">
         <v>1</v>
       </c>
       <c r="D1217" t="n">
-        <v>0.252</v>
+        <v>0.136</v>
       </c>
       <c r="E1217" t="n">
-        <v>0.264</v>
+        <v>0.194</v>
       </c>
       <c r="F1217" t="n">
-        <v>0.5116279069767442</v>
+        <v>0.5878787878787879</v>
       </c>
       <c r="G1217" t="n">
-        <v>0.4883720930232558</v>
+        <v>0.4121212121212121</v>
       </c>
       <c r="H1217" t="n">
-        <v>0.516</v>
+        <v>0.33</v>
       </c>
       <c r="I1217" t="n">
-        <v>0.01200000000000001</v>
+        <v>0.058</v>
       </c>
       <c r="J1217" t="n">
-        <v>0.02325581395348839</v>
+        <v>0.1757575757575757</v>
       </c>
       <c r="K1217" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -47615,36 +47615,36 @@
       </c>
       <c r="B1218" t="inlineStr">
         <is>
-          <t>few_modifiers_thres=11_label=1</t>
+          <t>low_num_words_in_sents_avg_thres=35_label=1</t>
         </is>
       </c>
       <c r="C1218" t="n">
         <v>1</v>
       </c>
       <c r="D1218" t="n">
-        <v>0.232</v>
+        <v>0.068</v>
       </c>
       <c r="E1218" t="n">
-        <v>0.248</v>
+        <v>0.114</v>
       </c>
       <c r="F1218" t="n">
-        <v>0.5166666666666667</v>
+        <v>0.6263736263736264</v>
       </c>
       <c r="G1218" t="n">
-        <v>0.4833333333333333</v>
+        <v>0.3736263736263736</v>
       </c>
       <c r="H1218" t="n">
-        <v>0.48</v>
+        <v>0.182</v>
       </c>
       <c r="I1218" t="n">
-        <v>0.01599999999999999</v>
+        <v>0.046</v>
       </c>
       <c r="J1218" t="n">
-        <v>0.03333333333333331</v>
+        <v>0.2527472527472527</v>
       </c>
       <c r="K1218" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -47654,36 +47654,36 @@
       </c>
       <c r="B1219" t="inlineStr">
         <is>
-          <t>few_modifiers_thres=12_label=1</t>
+          <t>low_num_words_in_sents_avg_thres=40_label=1</t>
         </is>
       </c>
       <c r="C1219" t="n">
         <v>1</v>
       </c>
       <c r="D1219" t="n">
-        <v>0.228</v>
+        <v>0.034</v>
       </c>
       <c r="E1219" t="n">
-        <v>0.242</v>
+        <v>0.068</v>
       </c>
       <c r="F1219" t="n">
-        <v>0.5148936170212766</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G1219" t="n">
-        <v>0.4851063829787234</v>
+        <v>0.3333333333333334</v>
       </c>
       <c r="H1219" t="n">
-        <v>0.47</v>
+        <v>0.102</v>
       </c>
       <c r="I1219" t="n">
-        <v>0.01399999999999998</v>
+        <v>0.034</v>
       </c>
       <c r="J1219" t="n">
-        <v>0.02978723404255316</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="K1219" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -47693,36 +47693,36 @@
       </c>
       <c r="B1220" t="inlineStr">
         <is>
-          <t>few_modifiers_thres=13_label=1</t>
+          <t>low_num_words_in_sents_avg_thres=42_label=1</t>
         </is>
       </c>
       <c r="C1220" t="n">
         <v>1</v>
       </c>
       <c r="D1220" t="n">
-        <v>0.22</v>
+        <v>0.028</v>
       </c>
       <c r="E1220" t="n">
-        <v>0.238</v>
+        <v>0.048</v>
       </c>
       <c r="F1220" t="n">
-        <v>0.5196506550218341</v>
+        <v>0.6315789473684211</v>
       </c>
       <c r="G1220" t="n">
-        <v>0.4803493449781659</v>
+        <v>0.3684210526315789</v>
       </c>
       <c r="H1220" t="n">
-        <v>0.458</v>
+        <v>0.076</v>
       </c>
       <c r="I1220" t="n">
-        <v>0.01799999999999999</v>
+        <v>0.02</v>
       </c>
       <c r="J1220" t="n">
-        <v>0.0393013100436681</v>
+        <v>0.2631578947368421</v>
       </c>
       <c r="K1220" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -47732,36 +47732,36 @@
       </c>
       <c r="B1221" t="inlineStr">
         <is>
-          <t>few_noun_phrases_thres=9_label=1</t>
+          <t>low_num_words_in_sents_avg_thres=45_label=1</t>
         </is>
       </c>
       <c r="C1221" t="n">
         <v>1</v>
       </c>
       <c r="D1221" t="n">
-        <v>0.476</v>
+        <v>0.018</v>
       </c>
       <c r="E1221" t="n">
-        <v>0.466</v>
+        <v>0.036</v>
       </c>
       <c r="F1221" t="n">
-        <v>0.4946921443736731</v>
+        <v>0.6666666666666667</v>
       </c>
       <c r="G1221" t="n">
-        <v>0.5053078556263269</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="H1221" t="n">
-        <v>0.9419999999999999</v>
+        <v>0.05399999999999999</v>
       </c>
       <c r="I1221" t="n">
-        <v>0.009999999999999953</v>
+        <v>0.018</v>
       </c>
       <c r="J1221" t="n">
-        <v>0.01061571125265388</v>
+        <v>0.3333333333333334</v>
       </c>
       <c r="K1221" t="inlineStr">
         <is>
-          <t>NEIN</t>
+          <t>JA</t>
         </is>
       </c>
     </row>
@@ -47771,32 +47771,32 @@
       </c>
       <c r="B1222" t="inlineStr">
         <is>
-          <t>few_noun_phrases_thres=10_label=1</t>
+          <t>low_num_words_in_sents_avg_thres=50_label=1</t>
         </is>
       </c>
       <c r="C1222" t="n">
         <v>1</v>
       </c>
       <c r="D1222" t="n">
-        <v>0.44</v>
+        <v>0.004</v>
       </c>
       <c r="E1222" t="n">
-        <v>0.428</v>
+        <v>0.01</v>
       </c>
       <c r="F1222" t="n">
-        <v>0.4930875576036866</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="G1222" t="n">
-        <v>0.5069124423963134</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="H1222" t="n">
-        <v>0.868</v>
+        <v>0.014</v>
       </c>
       <c r="I1222" t="n">
-        <v>0.01200000000000001</v>
+        <v>0.006</v>
       </c>
       <c r="J1222" t="n">
-        <v>0.01382488479262674</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="K1222" t="inlineStr">
         <is>
@@ -47810,32 +47810,32 @@
       </c>
       <c r="B1223" t="inlineStr">
         <is>
-          <t>few_noun_phrases_thres=11_label=1</t>
+          <t>num_sents_num_thres=5_label=1</t>
         </is>
       </c>
       <c r="C1223" t="n">
         <v>1</v>
       </c>
       <c r="D1223" t="n">
-        <v>0.4</v>
+        <v>0.208</v>
       </c>
       <c r="E1223" t="n">
-        <v>0.39</v>
+        <v>0.208</v>
       </c>
       <c r="F1223" t="n">
-        <v>0.4936708860759494</v>
+        <v>0.5</v>
       </c>
       <c r="G1223" t="n">
-        <v>0.5063291139240507</v>
+        <v>0.5</v>
       </c>
       <c r="H1223" t="n">
-        <v>0.79</v>
+        <v>0.416</v>
       </c>
       <c r="I1223" t="n">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
       <c r="J1223" t="n">
-        <v>0.01265822784810128</v>
+        <v>0</v>
       </c>
       <c r="K1223" t="inlineStr">
         <is>
@@ -47849,32 +47849,32 @@
       </c>
       <c r="B1224" t="inlineStr">
         <is>
-          <t>few_noun_phrases_thres=12_label=1</t>
+          <t>num_sents_num_thres=6_label=1</t>
         </is>
       </c>
       <c r="C1224" t="n">
         <v>1</v>
       </c>
       <c r="D1224" t="n">
-        <v>0.374</v>
+        <v>0.206</v>
       </c>
       <c r="E1224" t="n">
-        <v>0.37</v>
+        <v>0.208</v>
       </c>
       <c r="F1224" t="n">
-        <v>0.4973118279569892</v>
+        <v>0.5024154589371981</v>
       </c>
       <c r="G1224" t="n">
-        <v>0.5026881720430108</v>
+        <v>0.4975845410628019</v>
       </c>
       <c r="H1224" t="n">
-        <v>0.744</v>
+        <v>0.414</v>
       </c>
       <c r="I1224" t="n">
-        <v>0.004000000000000004</v>
+        <v>0.002000000000000002</v>
       </c>
       <c r="J1224" t="n">
-        <v>0.00537634408602151</v>
+        <v>0.004830917874396139</v>
       </c>
       <c r="K1224" t="inlineStr">
         <is>
@@ -47888,32 +47888,32 @@
       </c>
       <c r="B1225" t="inlineStr">
         <is>
-          <t>few_noun_phrases_thres=13_label=1</t>
+          <t>num_sents_num_thres=7_label=1</t>
         </is>
       </c>
       <c r="C1225" t="n">
         <v>1</v>
       </c>
       <c r="D1225" t="n">
-        <v>0.346</v>
+        <v>0.202</v>
       </c>
       <c r="E1225" t="n">
-        <v>0.334</v>
+        <v>0.204</v>
       </c>
       <c r="F1225" t="n">
-        <v>0.4911764705882354</v>
+        <v>0.5024630541871921</v>
       </c>
       <c r="G1225" t="n">
-        <v>0.5088235294117647</v>
+        <v>0.4975369458128079</v>
       </c>
       <c r="H1225" t="n">
-        <v>0.6799999999999999</v>
+        <v>0.406</v>
       </c>
       <c r="I1225" t="n">
-        <v>0.01199999999999996</v>
+        <v>0.001999999999999974</v>
       </c>
       <c r="J1225" t="n">
-        <v>0.01764705882352935</v>
+        <v>0.004926108374384172</v>
       </c>
       <c r="K1225" t="inlineStr">
         <is>
@@ -47927,32 +47927,32 @@
       </c>
       <c r="B1226" t="inlineStr">
         <is>
-          <t>few_noun_phrases_thres=14_label=1</t>
+          <t>num_sents_num_thres=8_label=1</t>
         </is>
       </c>
       <c r="C1226" t="n">
         <v>1</v>
       </c>
       <c r="D1226" t="n">
-        <v>0.318</v>
+        <v>0.202</v>
       </c>
       <c r="E1226" t="n">
-        <v>0.324</v>
+        <v>0.204</v>
       </c>
       <c r="F1226" t="n">
-        <v>0.5046728971962617</v>
+        <v>0.5024630541871921</v>
       </c>
       <c r="G1226" t="n">
-        <v>0.4953271028037383</v>
+        <v>0.4975369458128079</v>
       </c>
       <c r="H1226" t="n">
-        <v>0.642</v>
+        <v>0.406</v>
       </c>
       <c r="I1226" t="n">
-        <v>0.006000000000000005</v>
+        <v>0.001999999999999974</v>
       </c>
       <c r="J1226" t="n">
-        <v>0.009345794392523372</v>
+        <v>0.004926108374384172</v>
       </c>
       <c r="K1226" t="inlineStr">
         <is>
@@ -47966,32 +47966,32 @@
       </c>
       <c r="B1227" t="inlineStr">
         <is>
-          <t>few_noun_phrases_thres=15_label=1</t>
+          <t>num_sents_num_thres=9_label=1</t>
         </is>
       </c>
       <c r="C1227" t="n">
         <v>1</v>
       </c>
       <c r="D1227" t="n">
-        <v>0.304</v>
+        <v>0.202</v>
       </c>
       <c r="E1227" t="n">
-        <v>0.3</v>
+        <v>0.204</v>
       </c>
       <c r="F1227" t="n">
-        <v>0.4966887417218543</v>
+        <v>0.5024630541871921</v>
       </c>
       <c r="G1227" t="n">
-        <v>0.5033112582781457</v>
+        <v>0.4975369458128079</v>
       </c>
       <c r="H1227" t="n">
-        <v>0.604</v>
+        <v>0.406</v>
       </c>
       <c r="I1227" t="n">
-        <v>0.004000000000000004</v>
+        <v>0.001999999999999974</v>
       </c>
       <c r="J1227" t="n">
-        <v>0.006622516556291397</v>
+        <v>0.004926108374384172</v>
       </c>
       <c r="K1227" t="inlineStr">
         <is>
@@ -48005,32 +48005,32 @@
       </c>
       <c r="B1228" t="inlineStr">
         <is>
-          <t>few_noun_phrases_thres=16_label=1</t>
+          <t>num_sents_num_thres=10_label=1</t>
         </is>
       </c>
       <c r="C1228" t="n">
         <v>1</v>
       </c>
       <c r="D1228" t="n">
-        <v>0.284</v>
+        <v>0.196</v>
       </c>
       <c r="E1228" t="n">
-        <v>0.29</v>
+        <v>0.204</v>
       </c>
       <c r="F1228" t="n">
-        <v>0.5052264808362369</v>
+        <v>0.5099999999999999</v>
       </c>
       <c r="G1228" t="n">
-        <v>0.4947735191637631</v>
+        <v>0.4900000000000001</v>
       </c>
       <c r="H1228" t="n">
-        <v>0.574</v>
+        <v>0.4</v>
       </c>
       <c r="I1228" t="n">
-        <v>0.006000000000000005</v>
+        <v>0.007999999999999979</v>
       </c>
       <c r="J1228" t="n">
-        <v>0.01045296167247388</v>
+        <v>0.01999999999999995</v>
       </c>
       <c r="K1228" t="inlineStr">
         <is>
@@ -48044,32 +48044,32 @@
       </c>
       <c r="B1229" t="inlineStr">
         <is>
-          <t>few_noun_phrases_thres=17_label=1</t>
+          <t>num_sents_num_thres=11_label=1</t>
         </is>
       </c>
       <c r="C1229" t="n">
         <v>1</v>
       </c>
       <c r="D1229" t="n">
-        <v>0.278</v>
+        <v>0.194</v>
       </c>
       <c r="E1229" t="n">
-        <v>0.276</v>
+        <v>0.204</v>
       </c>
       <c r="F1229" t="n">
-        <v>0.4981949458483754</v>
+        <v>0.5125628140703516</v>
       </c>
       <c r="G1229" t="n">
-        <v>0.5018050541516246</v>
+        <v>0.4874371859296484</v>
       </c>
       <c r="H1229" t="n">
-        <v>0.554</v>
+        <v>0.398</v>
       </c>
       <c r="I1229" t="n">
-        <v>0.002000000000000002</v>
+        <v>0.009999999999999981</v>
       </c>
       <c r="J1229" t="n">
-        <v>0.0036101083032491</v>
+        <v>0.02512562814070347</v>
       </c>
       <c r="K1229" t="inlineStr">
         <is>
@@ -48083,32 +48083,32 @@
       </c>
       <c r="B1230" t="inlineStr">
         <is>
-          <t>few_noun_phrases_thres=18_label=1</t>
+          <t>few_modifiers_thres=5_label=1</t>
         </is>
       </c>
       <c r="C1230" t="n">
         <v>1</v>
       </c>
       <c r="D1230" t="n">
-        <v>0.256</v>
+        <v>0.432</v>
       </c>
       <c r="E1230" t="n">
-        <v>0.268</v>
+        <v>0.414</v>
       </c>
       <c r="F1230" t="n">
-        <v>0.5114503816793893</v>
+        <v>0.4893617021276596</v>
       </c>
       <c r="G1230" t="n">
-        <v>0.4885496183206107</v>
+        <v>0.5106382978723405</v>
       </c>
       <c r="H1230" t="n">
-        <v>0.524</v>
+        <v>0.846</v>
       </c>
       <c r="I1230" t="n">
-        <v>0.01200000000000001</v>
+        <v>0.01800000000000002</v>
       </c>
       <c r="J1230" t="n">
-        <v>0.02290076335877865</v>
+        <v>0.02127659574468087</v>
       </c>
       <c r="K1230" t="inlineStr">
         <is>
@@ -48122,32 +48122,32 @@
       </c>
       <c r="B1231" t="inlineStr">
         <is>
-          <t>few_noun_phrases_thres=19_label=1</t>
+          <t>few_modifiers_thres=6_label=1</t>
         </is>
       </c>
       <c r="C1231" t="n">
         <v>1</v>
       </c>
       <c r="D1231" t="n">
-        <v>0.244</v>
+        <v>0.364</v>
       </c>
       <c r="E1231" t="n">
-        <v>0.262</v>
+        <v>0.354</v>
       </c>
       <c r="F1231" t="n">
-        <v>0.5177865612648221</v>
+        <v>0.4930362116991643</v>
       </c>
       <c r="G1231" t="n">
-        <v>0.4822134387351779</v>
+        <v>0.5069637883008357</v>
       </c>
       <c r="H1231" t="n">
-        <v>0.506</v>
+        <v>0.718</v>
       </c>
       <c r="I1231" t="n">
-        <v>0.01800000000000002</v>
+        <v>0.01000000000000001</v>
       </c>
       <c r="J1231" t="n">
-        <v>0.0355731225296443</v>
+        <v>0.01392757660167132</v>
       </c>
       <c r="K1231" t="inlineStr">
         <is>
@@ -48161,34 +48161,736 @@
       </c>
       <c r="B1232" t="inlineStr">
         <is>
+          <t>few_modifiers_thres=7_label=1</t>
+        </is>
+      </c>
+      <c r="C1232" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1232" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="E1232" t="n">
+        <v>0.324</v>
+      </c>
+      <c r="F1232" t="n">
+        <v>0.5031055900621118</v>
+      </c>
+      <c r="G1232" t="n">
+        <v>0.4968944099378882</v>
+      </c>
+      <c r="H1232" t="n">
+        <v>0.644</v>
+      </c>
+      <c r="I1232" t="n">
+        <v>0.004000000000000004</v>
+      </c>
+      <c r="J1232" t="n">
+        <v>0.006211180124223608</v>
+      </c>
+      <c r="K1232" t="inlineStr">
+        <is>
+          <t>NEIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" s="1" t="n">
+        <v>1231</v>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>few_modifiers_thres=8_label=1</t>
+        </is>
+      </c>
+      <c r="C1233" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1233" t="n">
+        <v>0.296</v>
+      </c>
+      <c r="E1233" t="n">
+        <v>0.304</v>
+      </c>
+      <c r="F1233" t="n">
+        <v>0.5066666666666667</v>
+      </c>
+      <c r="G1233" t="n">
+        <v>0.4933333333333333</v>
+      </c>
+      <c r="H1233" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I1233" t="n">
+        <v>0.008000000000000007</v>
+      </c>
+      <c r="J1233" t="n">
+        <v>0.01333333333333335</v>
+      </c>
+      <c r="K1233" t="inlineStr">
+        <is>
+          <t>NEIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" s="1" t="n">
+        <v>1232</v>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>few_modifiers_thres=9_label=1</t>
+        </is>
+      </c>
+      <c r="C1234" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1234" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="E1234" t="n">
+        <v>0.276</v>
+      </c>
+      <c r="F1234" t="n">
+        <v>0.5054945054945055</v>
+      </c>
+      <c r="G1234" t="n">
+        <v>0.4945054945054945</v>
+      </c>
+      <c r="H1234" t="n">
+        <v>0.546</v>
+      </c>
+      <c r="I1234" t="n">
+        <v>0.006000000000000005</v>
+      </c>
+      <c r="J1234" t="n">
+        <v>0.010989010989011</v>
+      </c>
+      <c r="K1234" t="inlineStr">
+        <is>
+          <t>NEIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" s="1" t="n">
+        <v>1233</v>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>few_modifiers_thres=10_label=1</t>
+        </is>
+      </c>
+      <c r="C1235" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1235" t="n">
+        <v>0.252</v>
+      </c>
+      <c r="E1235" t="n">
+        <v>0.264</v>
+      </c>
+      <c r="F1235" t="n">
+        <v>0.5116279069767442</v>
+      </c>
+      <c r="G1235" t="n">
+        <v>0.4883720930232558</v>
+      </c>
+      <c r="H1235" t="n">
+        <v>0.516</v>
+      </c>
+      <c r="I1235" t="n">
+        <v>0.01200000000000001</v>
+      </c>
+      <c r="J1235" t="n">
+        <v>0.02325581395348839</v>
+      </c>
+      <c r="K1235" t="inlineStr">
+        <is>
+          <t>NEIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" s="1" t="n">
+        <v>1234</v>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>few_modifiers_thres=11_label=1</t>
+        </is>
+      </c>
+      <c r="C1236" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1236" t="n">
+        <v>0.232</v>
+      </c>
+      <c r="E1236" t="n">
+        <v>0.248</v>
+      </c>
+      <c r="F1236" t="n">
+        <v>0.5166666666666667</v>
+      </c>
+      <c r="G1236" t="n">
+        <v>0.4833333333333333</v>
+      </c>
+      <c r="H1236" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="I1236" t="n">
+        <v>0.01599999999999999</v>
+      </c>
+      <c r="J1236" t="n">
+        <v>0.03333333333333331</v>
+      </c>
+      <c r="K1236" t="inlineStr">
+        <is>
+          <t>NEIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" s="1" t="n">
+        <v>1235</v>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>few_modifiers_thres=12_label=1</t>
+        </is>
+      </c>
+      <c r="C1237" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1237" t="n">
+        <v>0.228</v>
+      </c>
+      <c r="E1237" t="n">
+        <v>0.242</v>
+      </c>
+      <c r="F1237" t="n">
+        <v>0.5148936170212766</v>
+      </c>
+      <c r="G1237" t="n">
+        <v>0.4851063829787234</v>
+      </c>
+      <c r="H1237" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="I1237" t="n">
+        <v>0.01399999999999998</v>
+      </c>
+      <c r="J1237" t="n">
+        <v>0.02978723404255316</v>
+      </c>
+      <c r="K1237" t="inlineStr">
+        <is>
+          <t>NEIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" s="1" t="n">
+        <v>1236</v>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>few_modifiers_thres=13_label=1</t>
+        </is>
+      </c>
+      <c r="C1238" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1238" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="E1238" t="n">
+        <v>0.238</v>
+      </c>
+      <c r="F1238" t="n">
+        <v>0.5196506550218341</v>
+      </c>
+      <c r="G1238" t="n">
+        <v>0.4803493449781659</v>
+      </c>
+      <c r="H1238" t="n">
+        <v>0.458</v>
+      </c>
+      <c r="I1238" t="n">
+        <v>0.01799999999999999</v>
+      </c>
+      <c r="J1238" t="n">
+        <v>0.0393013100436681</v>
+      </c>
+      <c r="K1238" t="inlineStr">
+        <is>
+          <t>NEIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" s="1" t="n">
+        <v>1237</v>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>few_noun_phrases_thres=9_label=1</t>
+        </is>
+      </c>
+      <c r="C1239" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1239" t="n">
+        <v>0.476</v>
+      </c>
+      <c r="E1239" t="n">
+        <v>0.466</v>
+      </c>
+      <c r="F1239" t="n">
+        <v>0.4946921443736731</v>
+      </c>
+      <c r="G1239" t="n">
+        <v>0.5053078556263269</v>
+      </c>
+      <c r="H1239" t="n">
+        <v>0.9419999999999999</v>
+      </c>
+      <c r="I1239" t="n">
+        <v>0.009999999999999953</v>
+      </c>
+      <c r="J1239" t="n">
+        <v>0.01061571125265388</v>
+      </c>
+      <c r="K1239" t="inlineStr">
+        <is>
+          <t>NEIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" s="1" t="n">
+        <v>1238</v>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>few_noun_phrases_thres=10_label=1</t>
+        </is>
+      </c>
+      <c r="C1240" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1240" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="E1240" t="n">
+        <v>0.428</v>
+      </c>
+      <c r="F1240" t="n">
+        <v>0.4930875576036866</v>
+      </c>
+      <c r="G1240" t="n">
+        <v>0.5069124423963134</v>
+      </c>
+      <c r="H1240" t="n">
+        <v>0.868</v>
+      </c>
+      <c r="I1240" t="n">
+        <v>0.01200000000000001</v>
+      </c>
+      <c r="J1240" t="n">
+        <v>0.01382488479262674</v>
+      </c>
+      <c r="K1240" t="inlineStr">
+        <is>
+          <t>NEIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" s="1" t="n">
+        <v>1239</v>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>few_noun_phrases_thres=11_label=1</t>
+        </is>
+      </c>
+      <c r="C1241" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1241" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E1241" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="F1241" t="n">
+        <v>0.4936708860759494</v>
+      </c>
+      <c r="G1241" t="n">
+        <v>0.5063291139240507</v>
+      </c>
+      <c r="H1241" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="I1241" t="n">
+        <v>0.01000000000000001</v>
+      </c>
+      <c r="J1241" t="n">
+        <v>0.01265822784810128</v>
+      </c>
+      <c r="K1241" t="inlineStr">
+        <is>
+          <t>NEIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" s="1" t="n">
+        <v>1240</v>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>few_noun_phrases_thres=12_label=1</t>
+        </is>
+      </c>
+      <c r="C1242" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1242" t="n">
+        <v>0.374</v>
+      </c>
+      <c r="E1242" t="n">
+        <v>0.37</v>
+      </c>
+      <c r="F1242" t="n">
+        <v>0.4973118279569892</v>
+      </c>
+      <c r="G1242" t="n">
+        <v>0.5026881720430108</v>
+      </c>
+      <c r="H1242" t="n">
+        <v>0.744</v>
+      </c>
+      <c r="I1242" t="n">
+        <v>0.004000000000000004</v>
+      </c>
+      <c r="J1242" t="n">
+        <v>0.00537634408602151</v>
+      </c>
+      <c r="K1242" t="inlineStr">
+        <is>
+          <t>NEIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" s="1" t="n">
+        <v>1241</v>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>few_noun_phrases_thres=13_label=1</t>
+        </is>
+      </c>
+      <c r="C1243" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1243" t="n">
+        <v>0.346</v>
+      </c>
+      <c r="E1243" t="n">
+        <v>0.334</v>
+      </c>
+      <c r="F1243" t="n">
+        <v>0.4911764705882354</v>
+      </c>
+      <c r="G1243" t="n">
+        <v>0.5088235294117647</v>
+      </c>
+      <c r="H1243" t="n">
+        <v>0.6799999999999999</v>
+      </c>
+      <c r="I1243" t="n">
+        <v>0.01199999999999996</v>
+      </c>
+      <c r="J1243" t="n">
+        <v>0.01764705882352935</v>
+      </c>
+      <c r="K1243" t="inlineStr">
+        <is>
+          <t>NEIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" s="1" t="n">
+        <v>1242</v>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>few_noun_phrases_thres=14_label=1</t>
+        </is>
+      </c>
+      <c r="C1244" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1244" t="n">
+        <v>0.318</v>
+      </c>
+      <c r="E1244" t="n">
+        <v>0.324</v>
+      </c>
+      <c r="F1244" t="n">
+        <v>0.5046728971962617</v>
+      </c>
+      <c r="G1244" t="n">
+        <v>0.4953271028037383</v>
+      </c>
+      <c r="H1244" t="n">
+        <v>0.642</v>
+      </c>
+      <c r="I1244" t="n">
+        <v>0.006000000000000005</v>
+      </c>
+      <c r="J1244" t="n">
+        <v>0.009345794392523372</v>
+      </c>
+      <c r="K1244" t="inlineStr">
+        <is>
+          <t>NEIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" s="1" t="n">
+        <v>1243</v>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>few_noun_phrases_thres=15_label=1</t>
+        </is>
+      </c>
+      <c r="C1245" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1245" t="n">
+        <v>0.304</v>
+      </c>
+      <c r="E1245" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="F1245" t="n">
+        <v>0.4966887417218543</v>
+      </c>
+      <c r="G1245" t="n">
+        <v>0.5033112582781457</v>
+      </c>
+      <c r="H1245" t="n">
+        <v>0.604</v>
+      </c>
+      <c r="I1245" t="n">
+        <v>0.004000000000000004</v>
+      </c>
+      <c r="J1245" t="n">
+        <v>0.006622516556291397</v>
+      </c>
+      <c r="K1245" t="inlineStr">
+        <is>
+          <t>NEIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" s="1" t="n">
+        <v>1244</v>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>few_noun_phrases_thres=16_label=1</t>
+        </is>
+      </c>
+      <c r="C1246" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1246" t="n">
+        <v>0.284</v>
+      </c>
+      <c r="E1246" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="F1246" t="n">
+        <v>0.5052264808362369</v>
+      </c>
+      <c r="G1246" t="n">
+        <v>0.4947735191637631</v>
+      </c>
+      <c r="H1246" t="n">
+        <v>0.574</v>
+      </c>
+      <c r="I1246" t="n">
+        <v>0.006000000000000005</v>
+      </c>
+      <c r="J1246" t="n">
+        <v>0.01045296167247388</v>
+      </c>
+      <c r="K1246" t="inlineStr">
+        <is>
+          <t>NEIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" s="1" t="n">
+        <v>1245</v>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>few_noun_phrases_thres=17_label=1</t>
+        </is>
+      </c>
+      <c r="C1247" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1247" t="n">
+        <v>0.278</v>
+      </c>
+      <c r="E1247" t="n">
+        <v>0.276</v>
+      </c>
+      <c r="F1247" t="n">
+        <v>0.4981949458483754</v>
+      </c>
+      <c r="G1247" t="n">
+        <v>0.5018050541516246</v>
+      </c>
+      <c r="H1247" t="n">
+        <v>0.554</v>
+      </c>
+      <c r="I1247" t="n">
+        <v>0.002000000000000002</v>
+      </c>
+      <c r="J1247" t="n">
+        <v>0.0036101083032491</v>
+      </c>
+      <c r="K1247" t="inlineStr">
+        <is>
+          <t>NEIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" s="1" t="n">
+        <v>1246</v>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>few_noun_phrases_thres=18_label=1</t>
+        </is>
+      </c>
+      <c r="C1248" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1248" t="n">
+        <v>0.256</v>
+      </c>
+      <c r="E1248" t="n">
+        <v>0.268</v>
+      </c>
+      <c r="F1248" t="n">
+        <v>0.5114503816793893</v>
+      </c>
+      <c r="G1248" t="n">
+        <v>0.4885496183206107</v>
+      </c>
+      <c r="H1248" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="I1248" t="n">
+        <v>0.01200000000000001</v>
+      </c>
+      <c r="J1248" t="n">
+        <v>0.02290076335877865</v>
+      </c>
+      <c r="K1248" t="inlineStr">
+        <is>
+          <t>NEIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" s="1" t="n">
+        <v>1247</v>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>few_noun_phrases_thres=19_label=1</t>
+        </is>
+      </c>
+      <c r="C1249" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1249" t="n">
+        <v>0.244</v>
+      </c>
+      <c r="E1249" t="n">
+        <v>0.262</v>
+      </c>
+      <c r="F1249" t="n">
+        <v>0.5177865612648221</v>
+      </c>
+      <c r="G1249" t="n">
+        <v>0.4822134387351779</v>
+      </c>
+      <c r="H1249" t="n">
+        <v>0.506</v>
+      </c>
+      <c r="I1249" t="n">
+        <v>0.01800000000000002</v>
+      </c>
+      <c r="J1249" t="n">
+        <v>0.0355731225296443</v>
+      </c>
+      <c r="K1249" t="inlineStr">
+        <is>
+          <t>NEIN</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" s="1" t="n">
+        <v>1248</v>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
           <t>few_noun_phrases_thres=20_label=1</t>
         </is>
       </c>
-      <c r="C1232" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1232" t="n">
+      <c r="C1250" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1250" t="n">
         <v>0.24</v>
       </c>
-      <c r="E1232" t="n">
+      <c r="E1250" t="n">
         <v>0.252</v>
       </c>
-      <c r="F1232" t="n">
+      <c r="F1250" t="n">
         <v>0.5121951219512195</v>
       </c>
-      <c r="G1232" t="n">
+      <c r="G1250" t="n">
         <v>0.4878048780487805</v>
       </c>
-      <c r="H1232" t="n">
+      <c r="H1250" t="n">
         <v>0.492</v>
       </c>
-      <c r="I1232" t="n">
+      <c r="I1250" t="n">
         <v>0.01200000000000001</v>
       </c>
-      <c r="J1232" t="n">
+      <c r="J1250" t="n">
         <v>0.02439024390243905</v>
       </c>
-      <c r="K1232" t="inlineStr">
+      <c r="K1250" t="inlineStr">
         <is>
           <t>NEIN</t>
         </is>

</xml_diff>